<commit_message>
Add reference PDFs and update theoretical framework docs
Added multiple new PDF references to the 'Referencias' folder and updated both the Marco.docx and Referencias.xlsx files in the 'Marco teórico' directory to include or reflect these new sources.
</commit_message>
<xml_diff>
--- a/Marco teórico/Referencias.xlsx
+++ b/Marco teórico/Referencias.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karen\Documents\HumanidadesDigitales_git\Marco teórico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D5C065-1C9C-4AAD-A93A-304F02C533D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6454AA1D-A9FE-45D6-B84A-CA08145B2789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
   <si>
     <t>Año</t>
   </si>
@@ -47,16 +47,7 @@
     <t>Autor(es)</t>
   </si>
   <si>
-    <t>Revista o fuente</t>
-  </si>
-  <si>
     <t>Tema central</t>
-  </si>
-  <si>
-    <t>Cita sugerida</t>
-  </si>
-  <si>
-    <t>Relevancia para tu tesis</t>
   </si>
   <si>
     <t>Link</t>
@@ -73,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve"> No trata ciencia, si no pedagogía politica. Contiene ejemplo de como se realiza un análisis de discurso con teorías del ACD.</t>
-  </si>
-  <si>
-    <t>Correspondencias y Análisis</t>
   </si>
   <si>
     <t>Es un análisis del discurso especifico de una columna de opinión colombiana.</t>
@@ -89,18 +77,12 @@
 Sánchez Mora, Ana María</t>
   </si>
   <si>
-    <t>Signo y Pensamiento</t>
-  </si>
-  <si>
     <t>Sobre comunicación del la ciencia. Los autores tienen otros articulos relacionados.</t>
   </si>
   <si>
     <t>https://revistas.javeriana.edu.co/index.php/signoypensamiento/article/view/39320</t>
   </si>
   <si>
-    <t>Posible utilidad</t>
-  </si>
-  <si>
     <t>Desafíos teóricos cruciales para la comunicación pública de la ciencia y la tecnología post pandemia en Iberoamérica.</t>
   </si>
   <si>
@@ -228,9 +210,6 @@
   </si>
   <si>
     <t>Kieran O'Halloran</t>
-  </si>
-  <si>
-    <t>Book</t>
   </si>
   <si>
     <t>El uso del lenguaje científico específico como estrategia argumentativa en la publicidad de la cosmética femenina</t>
@@ -276,6 +255,59 @@
   </si>
   <si>
     <t>Revisar bibliografía. Probablemente haré cosas como estas.</t>
+  </si>
+  <si>
+    <t>Relevancia para la tesis</t>
+  </si>
+  <si>
+    <t>( "scientific discourse" OR "scientific language" OR "science communication" ) AND ( "automatic detection" OR "automated identification" OR "text mining" OR "natural language processing" OR "NLP" ) AND ( "opinion texts" OR "editorials" OR "news articles" OR "media discourse" )</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>Más citado de la búsqueda en Scopus</t>
+  </si>
+  <si>
+    <t>Beyond Misinformation: Understanding and Coping with the
+“Post-Truth” Era</t>
+  </si>
+  <si>
+    <t>Stephan Lewandowsky; Ullrich K.H. Ecker; John Cook</t>
+  </si>
+  <si>
+    <t>Sobre la desconfianza en la ciencia, y los problemas de la desinformación. Epistemología alternativa.</t>
+  </si>
+  <si>
+    <t>( "scientific discourse" OR "scientific language" OR "science communication" ) AND ( "automatic detection" OR "automated identification" OR "text mining" OR "natural language processing" OR "NLP" OR "computational linguistics" ) AND ( "opinion texts" OR "editorials" OR "news articles" OR "media discourse" ) AND NOT ( "fake news" )</t>
+  </si>
+  <si>
+    <t>Automatic text summarization: A comprehensive survey</t>
+  </si>
+  <si>
+    <t>Wafaa S. El-Kassas a,⇑, Cherif R. Salama a,b, Ahmed A. Rafea b, Hoda K. Mohamed a</t>
+  </si>
+  <si>
+    <t>Métodos de procesamiento de lenguaje natural</t>
+  </si>
+  <si>
+    <t>Muy citado</t>
+  </si>
+  <si>
+    <t>Argument mining: A survey</t>
+  </si>
+  <si>
+    <t>Lawrence, John;
+Reed, Chris</t>
+  </si>
+  <si>
+    <t>Computational Paralinguistics: Emotion, Affect and Personality in Speech and Language Processing</t>
+  </si>
+  <si>
+    <t>LIBRO con métodos</t>
+  </si>
+  <si>
+    <t>text mining AND media analysis AND scientific discourse</t>
   </si>
 </sst>
 </file>
@@ -319,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -327,14 +359,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -354,22 +383,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -431,19 +444,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0FB6EDA7-1E30-4FFA-9BB1-20EE81422F3F}" name="Tabla1" displayName="Tabla1" ref="A1:J21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:J21" xr:uid="{0FB6EDA7-1E30-4FFA-9BB1-20EE81422F3F}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{2E679BF1-1847-4028-B1F7-86C3366CAADD}" name="Título" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{56407ADA-CFB9-4F7A-B2B3-F6A6073250E3}" name="Autor(es)" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{04CF9E76-61ED-4F9F-AA47-71151B2F533D}" name="Año" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{0354F460-D808-4D5E-BE41-7B0C7DB27ECE}" name="Revista o fuente" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{55574FCC-A792-4926-BFA5-A4779000E41F}" name="Tema central" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{F6CCE7BC-7926-49A1-ADD1-83F619BAA08D}" name="Cita sugerida" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{9C6033F1-6D8B-4E2F-AE6B-746E835C568B}" name="Relevancia para tu tesis" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{08740982-1F26-4ECD-926B-A9D90FABCA85}" name="Link" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{2C63FE2D-4EF4-487D-A910-40ECA396D572}" name="Posible utilidad" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{FFC76DC3-23E0-450C-BD82-02E6192C0C51}" name="Ecuación búsqueda" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0FB6EDA7-1E30-4FFA-9BB1-20EE81422F3F}" name="Tabla1" displayName="Tabla1" ref="A1:H26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:H26" xr:uid="{0FB6EDA7-1E30-4FFA-9BB1-20EE81422F3F}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{2E679BF1-1847-4028-B1F7-86C3366CAADD}" name="Título" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{56407ADA-CFB9-4F7A-B2B3-F6A6073250E3}" name="Autor(es)" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{04CF9E76-61ED-4F9F-AA47-71151B2F533D}" name="Año" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{55574FCC-A792-4926-BFA5-A4779000E41F}" name="Tema central" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{9C6033F1-6D8B-4E2F-AE6B-746E835C568B}" name="Relevancia para la tesis" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{08740982-1F26-4ECD-926B-A9D90FABCA85}" name="Link" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{2C63FE2D-4EF4-487D-A910-40ECA396D572}" name="Nota" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{FFC76DC3-23E0-450C-BD82-02E6192C0C51}" name="Ecuación búsqueda" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -688,11 +699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7F9960-2A60-4750-8843-174FA41E0DE2}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,17 +711,15 @@
     <col min="1" max="1" width="25.44140625" style="2"/>
     <col min="2" max="2" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15" style="2" customWidth="1"/>
-    <col min="10" max="10" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="25.44140625" style="2"/>
+    <col min="4" max="4" width="19.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="25.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -724,368 +733,387 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="2">
         <v>2014</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>2024</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2">
         <v>2021</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2">
         <v>2020</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2">
         <v>2023</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2">
         <v>2023</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2">
         <v>2016</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2">
         <v>2023</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="F9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2">
         <v>2019</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2">
         <v>2019</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="E11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2">
         <v>2019</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2">
         <v>2022</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="E13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2">
         <v>2023</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2">
         <v>2014</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2">
         <v>2017</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2">
         <v>2018</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2">
         <v>2025</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2">
         <v>2008</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C20" s="2">
         <v>2022</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C21" s="2">
         <v>2020</v>
       </c>
+      <c r="E21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="G21" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J21" s="3"/>
+      <c r="G22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="216" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="216" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2019</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="216" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H26" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>